<commit_message>
solve the planning problem with 729 scenario but we found that it is solved too fast. we will try larger problems
</commit_message>
<xml_diff>
--- a/planning/good_gap/Iteration.xlsx
+++ b/planning/good_gap/Iteration.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,9 +29,6 @@
     <t>Iterations</t>
   </si>
   <si>
-    <t>lb</t>
-  </si>
-  <si>
     <t>scenario 1 disjunction</t>
   </si>
   <si>
@@ -51,19 +48,27 @@
   </si>
   <si>
     <t>scenario 3 disjunction</t>
+  </si>
+  <si>
+    <t>Lower bound</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
     </font>
   </fonts>
   <fills count="2">
@@ -74,7 +79,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -82,12 +87,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -368,98 +402,99 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>976.81100000000004</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
         <v>978.25</v>
       </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="C3" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>983.76900000000001</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>3</v>
+      <c r="E4" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>987.221</v>
       </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="C5" s="3" t="s">
         <v>3</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>